<commit_message>
PLScombind out of sample results staan!
</commit_message>
<xml_diff>
--- a/results_PLScombined_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
+++ b/results_PLScombined_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>RMSE_OutSample</t>
+          <t>RMSE_TestSample</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>R2_OutSample</t>
+          <t>R2_TestSample</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Adjusted_R2_OutSample</t>
+          <t>Adjusted_R2_TestSample</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -490,31 +490,31 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0001932605029317143</v>
+        <v>0.04967061671052313</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7408975325494723</v>
+        <v>0.8024266576305294</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7353611550398457</v>
+        <v>0.7982050050157972</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3567500002330899</v>
+        <v>0.07367127193719293</v>
       </c>
       <c r="F2" t="n">
-        <v>-123378.043559192</v>
+        <v>0.9637309116279517</v>
       </c>
       <c r="G2" t="n">
-        <v>-138424.2683834837</v>
+        <v>0.9603726627046139</v>
       </c>
       <c r="H2" t="n">
-        <v>1579.791894801286</v>
+        <v>131.0858086492545</v>
       </c>
       <c r="I2" t="n">
-        <v>-158.3400236170757</v>
+        <v>-252.1716172985091</v>
       </c>
       <c r="J2" t="n">
-        <v>-140.9368290003657</v>
+        <v>-234.7684226817991</v>
       </c>
     </row>
     <row r="3">
@@ -522,31 +522,31 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0001587108284114279</v>
+        <v>0.0430195623246154</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8241854677291988</v>
+        <v>0.8322296691693302</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8196580548810236</v>
+        <v>0.8279094031393559</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3567538515261502</v>
+        <v>0.06969859823890841</v>
       </c>
       <c r="F3" t="n">
-        <v>-123380.7322683342</v>
+        <v>0.9665727112180673</v>
       </c>
       <c r="G3" t="n">
-        <v>-141887.9921085843</v>
+        <v>0.9627884898465278</v>
       </c>
       <c r="H3" t="n">
-        <v>1626.795450907924</v>
+        <v>161.7198899650198</v>
       </c>
       <c r="I3" t="n">
-        <v>-262.3972285279098</v>
+        <v>-311.4397799300395</v>
       </c>
       <c r="J3" t="n">
-        <v>-241.5133949878579</v>
+        <v>-290.5559463899876</v>
       </c>
     </row>
     <row r="4">
@@ -554,31 +554,31 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0001504470716000162</v>
+        <v>0.04246927223592505</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8485483495174682</v>
+        <v>0.847015936123746</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8439786876494607</v>
+        <v>0.8424000376447212</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3567531715501907</v>
+        <v>0.07005820289497666</v>
       </c>
       <c r="F4" t="n">
-        <v>-123380.2729975412</v>
+        <v>0.9667131045806088</v>
       </c>
       <c r="G4" t="n">
-        <v>-145525.6296894076</v>
+        <v>0.9622321763510754</v>
       </c>
       <c r="H4" t="n">
-        <v>1636.072083932355</v>
+        <v>164.7879603469766</v>
       </c>
       <c r="I4" t="n">
-        <v>-292.3275733730727</v>
+        <v>-315.5759206939533</v>
       </c>
       <c r="J4" t="n">
-        <v>-267.9631009096788</v>
+        <v>-291.2114482305593</v>
       </c>
     </row>
     <row r="5">
@@ -586,31 +586,31 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>0.000143335294780072</v>
+        <v>0.0422367466578034</v>
       </c>
       <c r="C5" t="n">
-        <v>0.85529903190382</v>
+        <v>0.8541423743941738</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8502877429654241</v>
+        <v>0.8490910280528465</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3567472479364076</v>
+        <v>0.0697987185196205</v>
       </c>
       <c r="F5" t="n">
-        <v>-123376.1516820812</v>
+        <v>0.9669380016364926</v>
       </c>
       <c r="G5" t="n">
-        <v>-149350.2888783089</v>
+        <v>0.9617518058147659</v>
       </c>
       <c r="H5" t="n">
-        <v>1660.87337034762</v>
+        <v>166.5517374879095</v>
       </c>
       <c r="I5" t="n">
-        <v>-292.7223682434744</v>
+        <v>-317.103474975819</v>
       </c>
       <c r="J5" t="n">
-        <v>-264.8772568567385</v>
+        <v>-289.2583635890831</v>
       </c>
     </row>
     <row r="6">
@@ -618,31 +618,31 @@
         <v>9</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0001336140751763983</v>
+        <v>0.04037852781878488</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8728756481214182</v>
+        <v>0.8716163745054414</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8679012169609519</v>
+        <v>0.8665926674208717</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3567432902100238</v>
+        <v>0.06820949929607642</v>
       </c>
       <c r="F6" t="n">
-        <v>-123373.4040206507</v>
+        <v>0.9684479120228996</v>
       </c>
       <c r="G6" t="n">
-        <v>-153383.3941878359</v>
+        <v>0.9627685361870215</v>
       </c>
       <c r="H6" t="n">
-        <v>1683.954164927541</v>
+        <v>178.0131686143943</v>
       </c>
       <c r="I6" t="n">
-        <v>-312.9246882247606</v>
+        <v>-338.0263372287885</v>
       </c>
       <c r="J6" t="n">
-        <v>-281.5989379146827</v>
+        <v>-306.7005869187106</v>
       </c>
     </row>
     <row r="7">
@@ -650,31 +650,31 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0001296128262459821</v>
+        <v>0.03778366543972687</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8828592916734631</v>
+        <v>0.8826457640777204</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8777439768993786</v>
+        <v>0.8775211249544768</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3567429526625967</v>
+        <v>0.064231858796339</v>
       </c>
       <c r="F7" t="n">
-        <v>-123373.1697708839</v>
+        <v>0.9710139330818076</v>
       </c>
       <c r="G7" t="n">
-        <v>-157643.7724850184</v>
+        <v>0.965098409220952</v>
       </c>
       <c r="H7" t="n">
-        <v>1687.700306449646</v>
+        <v>186.4478464623334</v>
       </c>
       <c r="I7" t="n">
-        <v>-321.9749391027647</v>
+        <v>-352.8956929246668</v>
       </c>
       <c r="J7" t="n">
-        <v>-287.1685498693448</v>
+        <v>-318.0893036912469</v>
       </c>
     </row>
     <row r="8">
@@ -682,31 +682,31 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>0.000125683570328973</v>
+        <v>0.03655437199078362</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8918267248839796</v>
+        <v>0.8910743815879055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8866078388038208</v>
+        <v>0.8858191982434623</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3567423084397159</v>
+        <v>0.06363285793608846</v>
       </c>
       <c r="F8" t="n">
-        <v>-123372.7191616742</v>
+        <v>0.9713504582728413</v>
       </c>
       <c r="G8" t="n">
-        <v>-162147.316612486</v>
+        <v>0.9647849382937007</v>
       </c>
       <c r="H8" t="n">
-        <v>1693.481642582885</v>
+        <v>191.0822397680694</v>
       </c>
       <c r="I8" t="n">
-        <v>-336.7022923751899</v>
+        <v>-360.1644795361389</v>
       </c>
       <c r="J8" t="n">
-        <v>-298.415264218428</v>
+        <v>-321.877451379377</v>
       </c>
     </row>
     <row r="9">
@@ -714,31 +714,31 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0001242906261552134</v>
+        <v>0.03602200881466022</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8940177899427647</v>
+        <v>0.895574745970436</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8884152061511928</v>
+        <v>0.8900544682243797</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3567399456289269</v>
+        <v>0.06254077995352933</v>
       </c>
       <c r="F9" t="n">
-        <v>-123371.0744158503</v>
+        <v>0.9741104121661414</v>
       </c>
       <c r="G9" t="n">
-        <v>-166914.1595037974</v>
+        <v>0.9675003046340923</v>
       </c>
       <c r="H9" t="n">
-        <v>1696.759137225215</v>
+        <v>194.0576474689833</v>
       </c>
       <c r="I9" t="n">
-        <v>-335.0085761615534</v>
+        <v>-364.1152949379666</v>
       </c>
       <c r="J9" t="n">
-        <v>-293.2409090814496</v>
+        <v>-322.3476278578627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>